<commit_message>
Preference Logic Bug Fixed
</commit_message>
<xml_diff>
--- a/static/latest_schedule.xlsx
+++ b/static/latest_schedule.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Minal</t>
+          <t>Jonnah</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Minjung</t>
+          <t>Mandy</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>yujin</t>
+          <t>Sam</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sam</t>
+          <t>Minal</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Sam</t>
+          <t>Minal</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Minal</t>
+          <t>yujin</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Jonnah</t>
+          <t>Minjung</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Seoyoon</t>
+          <t>Mandy</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Fionna</t>
+          <t>Minjung</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Minjung</t>
+          <t>Fionna</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Mandy</t>
+          <t>Seoyoon</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Fionna</t>
+          <t>Sam</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Mandy</t>
+          <t>Sungwoo</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Sungwoo</t>
+          <t>Fionna</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Name Clean for Parsing Excel
</commit_message>
<xml_diff>
--- a/static/latest_schedule.xlsx
+++ b/static/latest_schedule.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Jonnah</t>
+          <t>Jonnah✅</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Mandy</t>
+          <t>Mandy✅</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jonnah</t>
+          <t>Jonnah✅</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Sam</t>
+          <t>Sam✅</t>
         </is>
       </c>
     </row>
@@ -548,7 +548,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Sungwoo</t>
+          <t>Sungwoo✅</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Minal</t>
+          <t>Minal✅</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>yujin</t>
+          <t>yujin✅</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Mandy</t>
+          <t>Mandy✅</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Minal</t>
+          <t>Fionna✅</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Fionna</t>
+          <t>Minal✅</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>yujin</t>
+          <t>Seoyoon</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Seoyoon</t>
+          <t>yujin✅</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Sam</t>
+          <t>Sam✅</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Sungwoo</t>
+          <t>Sungwoo✅</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Fionna</t>
+          <t>Fionna✅</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Final Working Version with Name Clean
</commit_message>
<xml_diff>
--- a/static/latest_schedule.xlsx
+++ b/static/latest_schedule.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Jonnah✅</t>
+          <t>Jonnah</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Mandy✅</t>
+          <t>Mandy</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jonnah✅</t>
+          <t>Jonnah</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Sam✅</t>
+          <t>Sam</t>
         </is>
       </c>
     </row>
@@ -548,7 +548,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Sungwoo✅</t>
+          <t>Sungwoo</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Minal✅</t>
+          <t>Minal</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>yujin✅</t>
+          <t>yujin</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Mandy✅</t>
+          <t>Mandy</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Fionna✅</t>
+          <t>Minal</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Minal✅</t>
+          <t>Fionna</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>yujin✅</t>
+          <t>yujin</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Sam✅</t>
+          <t>Sam</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Sungwoo✅</t>
+          <t>Sungwoo</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Fionna✅</t>
+          <t>Fionna</t>
         </is>
       </c>
     </row>

</xml_diff>